<commit_message>
plate detection and capture Delete profile
</commit_message>
<xml_diff>
--- a/RFID.xlsx
+++ b/RFID.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/327142c71604ce89/Tài liệu/Third year/Embedded Systems/test_GUI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dustin/Documents/Parking-lot-system/parking-lot-system/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_2BB1D69C5B6056CA1028ED93553088B35299F7A1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0354860-B6AA-4031-AD89-8A660718B210}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B8F524-E6B8-CF41-A823-8B3832D899CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -37,19 +37,13 @@
     <t>Phone number</t>
   </si>
   <si>
-    <t>Table</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Vo Chi Cong</t>
   </si>
   <si>
     <t>Male</t>
-  </si>
-  <si>
-    <t>Hoang Quoc Viet</t>
-  </si>
-  <si>
-    <t>30G8 - 8888</t>
-  </si>
-  <si>
-    <t>Vo Chi Cong</t>
   </si>
   <si>
     <t>34-F3 - 2836</t>
@@ -69,14 +63,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -421,20 +415,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.9140625" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.08203125" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -454,54 +444,37 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2">
-        <v>30</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2">
-        <v>18001088</v>
+        <v>18492423</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3">
-        <v>18492423</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>35</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4">
         <v>23423423</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update title and excel file
</commit_message>
<xml_diff>
--- a/RFID.xlsx
+++ b/RFID.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github_VSCode\parking-lot-system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7275F579-11E7-4092-9519-EDEC129EB246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEA58CE-E3B9-4FC9-B445-083A0431D684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3150" yWindow="2380" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -35,27 +35,6 @@
   </si>
   <si>
     <t>Phone number</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Hoang Quoc Viet</t>
-  </si>
-  <si>
-    <t>30G8 - 8888</t>
-  </si>
-  <si>
-    <t>Vo Chi Cong</t>
-  </si>
-  <si>
-    <t>34-F3 - 2836</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pham Van Dong </t>
-  </si>
-  <si>
-    <t>27-D9 - 9283</t>
   </si>
   <si>
     <t>Output_ID</t>
@@ -427,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -460,68 +439,11 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2">
-        <v>30</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2">
-        <v>18001088</v>
-      </c>
-      <c r="F2" s="3">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2">
-        <v>45</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2">
-        <v>18492423</v>
-      </c>
-      <c r="F3" s="2">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2">
-        <v>35</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="2">
-        <v>23423423</v>
-      </c>
-      <c r="F4" s="2">
-        <v>345</v>
-      </c>
+      <c r="F2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>